<commit_message>
จัดทำ test ของ Project Manager
</commit_message>
<xml_diff>
--- a/Employee/test_login/test_data.xlsx
+++ b/Employee/test_login/test_data.xlsx
@@ -5,29 +5,40 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automate Test\Test_PMS\automateTestTeam0\Admin\test_login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\automateTestTeam0\Employee\test_login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30962FBF-3CA4-4A79-AC2D-F478A385F64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8518FC8-9FB9-45EE-B38C-AB8DED17A5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
-    <sheet name="Project Manager" sheetId="4" r:id="rId2"/>
+    <sheet name="Project_Manager" sheetId="4" r:id="rId2"/>
     <sheet name="Admin" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -75,6 +86,18 @@
   </si>
   <si>
     <t>'</t>
+  </si>
+  <si>
+    <t>pol12@gmail.com</t>
+  </si>
+  <si>
+    <t>pol13@gmail.com</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>pol1234</t>
   </si>
 </sst>
 </file>
@@ -127,13 +150,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,18 +449,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="3" max="3" width="101.6328125" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="101.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -450,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>3</v>
@@ -459,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -467,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -478,7 +510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -489,7 +521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -500,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -525,18 +557,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850FD9B6-EE38-47DE-894F-A0E7C7A821D7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="3" max="3" width="101.6328125" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="101.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,28 +579,79 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
+      <c r="B3" s="5">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{C9F0AB97-6F91-4741-9A44-14D6FA47E239}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -581,14 +664,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="3" max="3" width="101.6328125" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="101.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,25 +682,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
     </row>
   </sheetData>

</xml_diff>